<commit_message>
unit9: 엑셀 with color
</commit_message>
<xml_diff>
--- a/etc/test.xlsx
+++ b/etc/test.xlsx
@@ -26,12 +26,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+        <bgColor rgb="00008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +441,21 @@
           <t>hello world</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>